<commit_message>
Fix analisi reticolo sodio
</commit_message>
<xml_diff>
--- a/Spettrometro/reticoloNa.xlsx
+++ b/Spettrometro/reticoloNa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ALL\Stefano\Bicocca\secondo_anno\lab2\Laboratorio_2\Spettrometro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesco\Desktop\Desktop Files\Uni\ANNO2\Laboratorio_2\Spettrometro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A893DCE9-69D0-4573-9758-B0693FF37E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF256482-1464-423B-A7DB-6B88D29CA16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2D61964-DCAF-4660-911B-25EFBBED7C6C}"/>
+    <workbookView xWindow="-28920" yWindow="3060" windowWidth="29040" windowHeight="15840" xr2:uid="{C2D61964-DCAF-4660-911B-25EFBBED7C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -54,14 +65,14 @@
     <t>^new (bad)^</t>
   </si>
   <si>
-    <t>^new(good)^</t>
+    <t>^new("good")^</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,21 +440,21 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1</v>
       </c>
@@ -507,7 +518,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -546,7 +557,7 @@
         <v>-10.199999999999989</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>1</v>
       </c>
@@ -577,7 +588,7 @@
         <v>-0.1907499999999942</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>2</v>
       </c>
@@ -608,7 +619,7 @@
         <v>-11.444999999999652</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>2</v>
       </c>
@@ -631,7 +642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>2</v>
       </c>
@@ -660,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>3</v>
       </c>
@@ -683,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>3</v>
       </c>
@@ -706,7 +717,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>3</v>
       </c>
@@ -729,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -752,7 +763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>1</v>
       </c>
@@ -784,7 +795,7 @@
         <v>211.2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>1</v>
       </c>
@@ -815,7 +826,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>2</v>
       </c>
@@ -842,7 +853,7 @@
         <v>8.0000000000012506E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>2</v>
       </c>
@@ -869,7 +880,7 @@
         <v>4.8000000000007503</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>3</v>
       </c>
@@ -892,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>3</v>
       </c>

</xml_diff>